<commit_message>
Latest generated NSW Sensitive list
</commit_message>
<xml_diff>
--- a/analysis/Monitoring/ListSources.xlsx
+++ b/analysis/Monitoring/ListSources.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oco115\PycharmProjects\authoritative-lists\analysis\Monitoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A22FA77-01E8-4D48-9B22-62B4AB522CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F153BA77-CD26-47A2-920F-88B43B4C1917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="4710" windowWidth="29790" windowHeight="13830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8565" yWindow="1335" windowWidth="20985" windowHeight="14055" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="69">
   <si>
     <t>List Type</t>
   </si>
@@ -309,6 +310,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>https://www.environment.act.gov.au/nature-conservation/conservation-and-ecological-communities/threatened-species-and-ecological-communities#threatened-species-act</t>
   </si>
 </sst>
 </file>
@@ -668,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="F7" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -872,6 +876,9 @@
       </c>
       <c r="E17" t="s">
         <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1022,4 +1029,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId33"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68722F78-0B03-4C38-BE6B-32D7733E1DF0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>